<commit_message>
move fixes for efforts
</commit_message>
<xml_diff>
--- a/data/schema.xlsx
+++ b/data/schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sgaliamov\projects\personal\ergo-balance\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A6D34B-4238-46BE-9327-C22315D14579}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCAA79A3-E49E-4CDE-B83B-31CA46547E8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="984" yWindow="-108" windowWidth="29844" windowHeight="17496" xr2:uid="{A7936750-1AB8-47D4-A3AD-A653CF22CC3F}"/>
   </bookViews>
@@ -170,7 +170,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-middle finger is mobile</t>
+middle finger is mobile but same finger</t>
         </r>
       </text>
     </comment>
@@ -587,7 +587,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>L</t>
   </si>
@@ -608,6 +608,9 @@
   </si>
   <si>
     <t>worst/ when need bend long finger and reach short</t>
+  </si>
+  <si>
+    <t>middle up 1, down 2, same +1, over row +2, +1 for bend</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1252,7 @@
   <dimension ref="A1:AF32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
@@ -1372,6 +1375,9 @@
       </c>
       <c r="T3" t="s">
         <v>3</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
@@ -1539,7 +1545,7 @@
       </c>
       <c r="AF8" t="str">
         <f>_xlfn.CONCAT("""0"": { ",_xlfn.TEXTJOIN(", ",TRUE,B12:F14),"}")</f>
-        <v>"0": { "0": 4, "1": 1, "2": 1, "3": 1, "4": 2, "5": 3, "6": 3, "7": 2, "8": 1, "9": 2, "10": 5, "11": 5, "12": 5, "13": 4, "14": 4}</v>
+        <v>"0": { "0": 4, "1": 1, "2": 1, "3": 1, "4": 2, "5": 3, "6": 3, "7": 2, "8": 1, "9": 3, "10": 5, "11": 5, "12": 5, "13": 4, "14": 4}</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
@@ -1556,7 +1562,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9" s="26">
         <v>1</v>
@@ -1580,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="P9" s="18">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="24">
         <v>1</v>
@@ -1607,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="AA9" s="22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB9" s="18">
         <v>2</v>
@@ -1701,7 +1707,7 @@
       </c>
       <c r="AF10" s="12" t="str">
         <f>_xlfn.CONCAT("""2"": { ",_xlfn.TEXTJOIN(", ",TRUE,N12:R14),"}")</f>
-        <v>"2": { "0": 4, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 2, "8": 1, "9": 3, "10": 4, "11": 4, "12": 5, "13": 4, "14": 4}</v>
+        <v>"2": { "0": 4, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 3, "8": 1, "9": 3, "10": 4, "11": 4, "12": 5, "13": 4, "14": 4}</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
@@ -1823,7 +1829,7 @@
       </c>
       <c r="AF12" s="12" t="str">
         <f>_xlfn.CONCAT("""4"": { ",_xlfn.TEXTJOIN(", ",TRUE,Z12:AD14),"}")</f>
-        <v>"4": { "0": 4, "1": 2, "2": 1, "3": 1, "4": 3, "5": 3, "6": 1, "7": 2, "8": 2, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}</v>
+        <v>"4": { "0": 4, "1": 2, "2": 1, "3": 1, "4": 3, "5": 3, "6": 2, "7": 2, "8": 2, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
@@ -1846,7 +1852,7 @@
       </c>
       <c r="F13" s="14" t="str">
         <f>_xlfn.CONCAT("""",$F$3, """: ", F9)</f>
-        <v>"9": 2</v>
+        <v>"9": 3</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14" t="str">
@@ -1880,7 +1886,7 @@
       </c>
       <c r="P13" s="14" t="str">
         <f>_xlfn.CONCAT("""",$D$3, """: ", P9)</f>
-        <v>"7": 2</v>
+        <v>"7": 3</v>
       </c>
       <c r="Q13" s="14" t="str">
         <f>_xlfn.CONCAT("""",$E$3, """: ", Q9)</f>
@@ -1918,7 +1924,7 @@
       </c>
       <c r="AA13" s="14" t="str">
         <f>_xlfn.CONCAT("""",$C$3, """: ", AA9)</f>
-        <v>"6": 1</v>
+        <v>"6": 2</v>
       </c>
       <c r="AB13" s="14" t="str">
         <f>_xlfn.CONCAT("""",$D$3, """: ", AB9)</f>
@@ -2041,7 +2047,7 @@
       </c>
       <c r="AF14" t="str">
         <f>_xlfn.TEXTJOIN(", ",TRUE,AF8:AF12)</f>
-        <v>"0": { "0": 4, "1": 1, "2": 1, "3": 1, "4": 2, "5": 3, "6": 3, "7": 2, "8": 1, "9": 2, "10": 5, "11": 5, "12": 5, "13": 4, "14": 4}, "1": { "0": 4, "1": 2, "2": 1, "3": 2, "4": 3, "5": 1, "6": 3, "7": 2, "8": 1, "9": 3, "10": 4, "11": 5, "12": 5, "13": 4, "14": 4}, "2": { "0": 4, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 2, "8": 1, "9": 3, "10": 4, "11": 4, "12": 5, "13": 4, "14": 4}, "3": { "0": 3, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 2, "8": 3, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}, "4": { "0": 4, "1": 2, "2": 1, "3": 1, "4": 3, "5": 3, "6": 1, "7": 2, "8": 2, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}</v>
+        <v>"0": { "0": 4, "1": 1, "2": 1, "3": 1, "4": 2, "5": 3, "6": 3, "7": 2, "8": 1, "9": 3, "10": 5, "11": 5, "12": 5, "13": 4, "14": 4}, "1": { "0": 4, "1": 2, "2": 1, "3": 2, "4": 3, "5": 1, "6": 3, "7": 2, "8": 1, "9": 3, "10": 4, "11": 5, "12": 5, "13": 4, "14": 4}, "2": { "0": 4, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 3, "8": 1, "9": 3, "10": 4, "11": 4, "12": 5, "13": 4, "14": 4}, "3": { "0": 3, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 2, "8": 3, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}, "4": { "0": 4, "1": 2, "2": 1, "3": 1, "4": 3, "5": 3, "6": 2, "7": 2, "8": 2, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
@@ -2108,7 +2114,7 @@
         <v>2</v>
       </c>
       <c r="V16" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W16" s="19">
         <v>3</v>
@@ -2135,7 +2141,7 @@
       <c r="AE16" s="12"/>
       <c r="AF16" s="12" t="str">
         <f>_xlfn.CONCAT("""5"": { ",_xlfn.TEXTJOIN(", ",TRUE,B20:F22),"}")</f>
-        <v>"5": { "0": 4, "1": 2, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 4, "11": 3, "12": 3, "13": 2, "14": 3}</v>
+        <v>"5": { "0": 4, "1": 2, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.3">
@@ -2228,7 +2234,7 @@
     <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18" s="12"/>
       <c r="B18" s="20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" s="17">
         <v>3</v>
@@ -2295,7 +2301,7 @@
         <v>4</v>
       </c>
       <c r="AA18" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB18" s="18">
         <v>3</v>
@@ -2346,7 +2352,7 @@
       <c r="AE19" s="12"/>
       <c r="AF19" s="12" t="str">
         <f>_xlfn.CONCAT("""8"": { ",_xlfn.TEXTJOIN(", ",TRUE,T20:X22),"}")</f>
-        <v>"8": { "0": 4, "1": 2, "2": 2, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 3, "10": 3, "11": 3, "12": 3, "13": 3, "14": 3}</v>
+        <v>"8": { "0": 4, "1": 2, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 3, "10": 3, "11": 3, "12": 3, "13": 3, "14": 3}</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.3">
@@ -2424,7 +2430,7 @@
       </c>
       <c r="V20" s="13" t="str">
         <f>_xlfn.CONCAT("""",$D$2, """: ", V16)</f>
-        <v>"2": 2</v>
+        <v>"2": 1</v>
       </c>
       <c r="W20" s="13" t="str">
         <f>_xlfn.CONCAT("""",$E$2, """: ", W16)</f>
@@ -2458,7 +2464,7 @@
       <c r="AE20" s="12"/>
       <c r="AF20" s="12" t="str">
         <f>_xlfn.CONCAT("""9"": { ",_xlfn.TEXTJOIN(", ",TRUE,Z20:AD22),"}")</f>
-        <v>"9": { "0": 5, "1": 4, "2": 3, "3": 2, "4": 3, "5": 2, "6": 1, "7": 1, "8": 1, "9": 2, "10": 4, "11": 4, "12": 3, "13": 3, "14": 3}</v>
+        <v>"9": { "0": 5, "1": 4, "2": 3, "3": 2, "4": 3, "5": 2, "6": 1, "7": 1, "8": 1, "9": 2, "10": 4, "11": 3, "12": 3, "13": 3, "14": 3}</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.3">
@@ -2573,7 +2579,7 @@
       <c r="A22" s="12"/>
       <c r="B22" s="13" t="str">
         <f>_xlfn.CONCAT("""",$B$4, """: ", B18)</f>
-        <v>"10": 4</v>
+        <v>"10": 3</v>
       </c>
       <c r="C22" s="13" t="str">
         <f>_xlfn.CONCAT("""",$C$4, """: ", C18)</f>
@@ -2661,7 +2667,7 @@
       </c>
       <c r="AA22" s="13" t="str">
         <f>_xlfn.CONCAT("""",$C$4, """: ", AA18)</f>
-        <v>"11": 4</v>
+        <v>"11": 3</v>
       </c>
       <c r="AB22" s="13" t="str">
         <f>_xlfn.CONCAT("""",$D$4, """: ", AB18)</f>
@@ -2678,7 +2684,7 @@
       <c r="AE22" s="12"/>
       <c r="AF22" s="12" t="str">
         <f>_xlfn.TEXTJOIN(", ",TRUE,AF16:AF20)</f>
-        <v>"5": { "0": 4, "1": 2, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 4, "11": 3, "12": 3, "13": 2, "14": 3}, "6": { "0": 5, "1": 3, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "7": { "0": 5, "1": 3, "2": 2, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "8": { "0": 4, "1": 2, "2": 2, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 3, "10": 3, "11": 3, "12": 3, "13": 3, "14": 3}, "9": { "0": 5, "1": 4, "2": 3, "3": 2, "4": 3, "5": 2, "6": 1, "7": 1, "8": 1, "9": 2, "10": 4, "11": 4, "12": 3, "13": 3, "14": 3}</v>
+        <v>"5": { "0": 4, "1": 2, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "6": { "0": 5, "1": 3, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "7": { "0": 5, "1": 3, "2": 2, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "8": { "0": 4, "1": 2, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 3, "10": 3, "11": 3, "12": 3, "13": 3, "14": 3}, "9": { "0": 5, "1": 4, "2": 3, "3": 2, "4": 3, "5": 2, "6": 1, "7": 1, "8": 1, "9": 2, "10": 4, "11": 3, "12": 3, "13": 3, "14": 3}</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.3">
@@ -2807,7 +2813,7 @@
         <v>3</v>
       </c>
       <c r="P25" s="18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q25" s="19">
         <v>2</v>
@@ -2936,7 +2942,7 @@
       <c r="AE26" s="12"/>
       <c r="AF26" s="12" t="str">
         <f>_xlfn.CONCAT("""12"": { ",_xlfn.TEXTJOIN(", ",TRUE,N28:R30),"}")</f>
-        <v>"12": { "0": 5, "1": 5, "2": 5, "3": 5, "4": 5, "5": 4, "6": 3, "7": 3, "8": 2, "9": 4, "10": 1, "11": 1, "12": 3, "13": 1, "14": 2}</v>
+        <v>"12": { "0": 5, "1": 5, "2": 5, "3": 5, "4": 5, "5": 4, "6": 3, "7": 2, "8": 2, "9": 4, "10": 1, "11": 1, "12": 3, "13": 1, "14": 2}</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.3">
@@ -3139,7 +3145,7 @@
       </c>
       <c r="P29" s="14" t="str">
         <f>_xlfn.CONCAT("""",$D$3, """: ", P25)</f>
-        <v>"7": 3</v>
+        <v>"7": 2</v>
       </c>
       <c r="Q29" s="14" t="str">
         <f>_xlfn.CONCAT("""",$E$3, """: ", Q25)</f>
@@ -3302,13 +3308,13 @@
       <c r="AE30" s="12"/>
       <c r="AF30" s="12" t="str">
         <f>_xlfn.TEXTJOIN(", ",TRUE,AF24:AF28)</f>
-        <v>"10": { "0": 5, "1": 4, "2": 3, "3": 4, "4": 5, "5": 3, "6": 2, "7": 1, "8": 2, "9": 4, "10": 3, "11": 1, "12": 1, "13": 1, "14": 2}, "11": { "0": 5, "1": 5, "2": 3, "3": 4, "4": 5, "5": 4, "6": 3, "7": 1, "8": 2, "9": 4, "10": 1, "11": 3, "12": 1, "13": 1, "14": 2}, "12": { "0": 5, "1": 5, "2": 5, "3": 5, "4": 5, "5": 4, "6": 3, "7": 3, "8": 2, "9": 4, "10": 1, "11": 1, "12": 3, "13": 1, "14": 2}, "13": { "0": 5, "1": 4, "2": 3, "3": 5, "4": 5, "5": 3, "6": 2, "7": 1, "8": 3, "9": 4, "10": 1, "11": 1, "12": 1, "13": 2, "14": 3}, "14": { "0": 5, "1": 5, "2": 4, "3": 3, "4": 5, "5": 3, "6": 3, "7": 1, "8": 1, "9": 3, "10": 2, "11": 1, "12": 1, "13": 1, "14": 3}</v>
+        <v>"10": { "0": 5, "1": 4, "2": 3, "3": 4, "4": 5, "5": 3, "6": 2, "7": 1, "8": 2, "9": 4, "10": 3, "11": 1, "12": 1, "13": 1, "14": 2}, "11": { "0": 5, "1": 5, "2": 3, "3": 4, "4": 5, "5": 4, "6": 3, "7": 1, "8": 2, "9": 4, "10": 1, "11": 3, "12": 1, "13": 1, "14": 2}, "12": { "0": 5, "1": 5, "2": 5, "3": 5, "4": 5, "5": 4, "6": 3, "7": 2, "8": 2, "9": 4, "10": 1, "11": 1, "12": 3, "13": 1, "14": 2}, "13": { "0": 5, "1": 4, "2": 3, "3": 5, "4": 5, "5": 3, "6": 2, "7": 1, "8": 3, "9": 4, "10": 1, "11": 1, "12": 1, "13": 2, "14": 3}, "14": { "0": 5, "1": 5, "2": 4, "3": 3, "4": 5, "5": 3, "6": 3, "7": 1, "8": 1, "9": 3, "10": 2, "11": 1, "12": 1, "13": 1, "14": 3}</v>
       </c>
     </row>
     <row r="32" spans="1:32" x14ac:dyDescent="0.3">
       <c r="B32" s="12" t="str">
         <f>_xlfn.CONCAT("{", _xlfn.TEXTJOIN(", ",TRUE,AF14, AF22, AF30),"}")</f>
-        <v>{"0": { "0": 4, "1": 1, "2": 1, "3": 1, "4": 2, "5": 3, "6": 3, "7": 2, "8": 1, "9": 2, "10": 5, "11": 5, "12": 5, "13": 4, "14": 4}, "1": { "0": 4, "1": 2, "2": 1, "3": 2, "4": 3, "5": 1, "6": 3, "7": 2, "8": 1, "9": 3, "10": 4, "11": 5, "12": 5, "13": 4, "14": 4}, "2": { "0": 4, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 2, "8": 1, "9": 3, "10": 4, "11": 4, "12": 5, "13": 4, "14": 4}, "3": { "0": 3, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 2, "8": 3, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}, "4": { "0": 4, "1": 2, "2": 1, "3": 1, "4": 3, "5": 3, "6": 1, "7": 2, "8": 2, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}, "5": { "0": 4, "1": 2, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 4, "11": 3, "12": 3, "13": 2, "14": 3}, "6": { "0": 5, "1": 3, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "7": { "0": 5, "1": 3, "2": 2, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "8": { "0": 4, "1": 2, "2": 2, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 3, "10": 3, "11": 3, "12": 3, "13": 3, "14": 3}, "9": { "0": 5, "1": 4, "2": 3, "3": 2, "4": 3, "5": 2, "6": 1, "7": 1, "8": 1, "9": 2, "10": 4, "11": 4, "12": 3, "13": 3, "14": 3}, "10": { "0": 5, "1": 4, "2": 3, "3": 4, "4": 5, "5": 3, "6": 2, "7": 1, "8": 2, "9": 4, "10": 3, "11": 1, "12": 1, "13": 1, "14": 2}, "11": { "0": 5, "1": 5, "2": 3, "3": 4, "4": 5, "5": 4, "6": 3, "7": 1, "8": 2, "9": 4, "10": 1, "11": 3, "12": 1, "13": 1, "14": 2}, "12": { "0": 5, "1": 5, "2": 5, "3": 5, "4": 5, "5": 4, "6": 3, "7": 3, "8": 2, "9": 4, "10": 1, "11": 1, "12": 3, "13": 1, "14": 2}, "13": { "0": 5, "1": 4, "2": 3, "3": 5, "4": 5, "5": 3, "6": 2, "7": 1, "8": 3, "9": 4, "10": 1, "11": 1, "12": 1, "13": 2, "14": 3}, "14": { "0": 5, "1": 5, "2": 4, "3": 3, "4": 5, "5": 3, "6": 3, "7": 1, "8": 1, "9": 3, "10": 2, "11": 1, "12": 1, "13": 1, "14": 3}}</v>
+        <v>{"0": { "0": 4, "1": 1, "2": 1, "3": 1, "4": 2, "5": 3, "6": 3, "7": 2, "8": 1, "9": 3, "10": 5, "11": 5, "12": 5, "13": 4, "14": 4}, "1": { "0": 4, "1": 2, "2": 1, "3": 2, "4": 3, "5": 1, "6": 3, "7": 2, "8": 1, "9": 3, "10": 4, "11": 5, "12": 5, "13": 4, "14": 4}, "2": { "0": 4, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 3, "8": 1, "9": 3, "10": 4, "11": 4, "12": 5, "13": 4, "14": 4}, "3": { "0": 3, "1": 1, "2": 1, "3": 2, "4": 3, "5": 1, "6": 2, "7": 2, "8": 3, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}, "4": { "0": 4, "1": 2, "2": 1, "3": 1, "4": 3, "5": 3, "6": 2, "7": 2, "8": 2, "9": 3, "10": 4, "11": 4, "12": 5, "13": 5, "14": 5}, "5": { "0": 4, "1": 2, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "6": { "0": 5, "1": 3, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "7": { "0": 5, "1": 3, "2": 2, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 2, "10": 3, "11": 3, "12": 3, "13": 2, "14": 3}, "8": { "0": 4, "1": 2, "2": 1, "3": 3, "4": 4, "5": 1, "6": 1, "7": 1, "8": 1, "9": 3, "10": 3, "11": 3, "12": 3, "13": 3, "14": 3}, "9": { "0": 5, "1": 4, "2": 3, "3": 2, "4": 3, "5": 2, "6": 1, "7": 1, "8": 1, "9": 2, "10": 4, "11": 3, "12": 3, "13": 3, "14": 3}, "10": { "0": 5, "1": 4, "2": 3, "3": 4, "4": 5, "5": 3, "6": 2, "7": 1, "8": 2, "9": 4, "10": 3, "11": 1, "12": 1, "13": 1, "14": 2}, "11": { "0": 5, "1": 5, "2": 3, "3": 4, "4": 5, "5": 4, "6": 3, "7": 1, "8": 2, "9": 4, "10": 1, "11": 3, "12": 1, "13": 1, "14": 2}, "12": { "0": 5, "1": 5, "2": 5, "3": 5, "4": 5, "5": 4, "6": 3, "7": 2, "8": 2, "9": 4, "10": 1, "11": 1, "12": 3, "13": 1, "14": 2}, "13": { "0": 5, "1": 4, "2": 3, "3": 5, "4": 5, "5": 3, "6": 2, "7": 1, "8": 3, "9": 4, "10": 1, "11": 1, "12": 1, "13": 2, "14": 3}, "14": { "0": 5, "1": 5, "2": 4, "3": 3, "4": 5, "5": 3, "6": 3, "7": 1, "8": 1, "9": 3, "10": 2, "11": 1, "12": 1, "13": 1, "14": 3}}</v>
       </c>
     </row>
   </sheetData>

</xml_diff>